<commit_message>
get named range working
</commit_message>
<xml_diff>
--- a/Test Open Xml/test.xlsx
+++ b/Test Open Xml/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tupp_js\Documents\LabVIEW Data\OpenXml LabVIEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Open-Xml-LabVIEW\Test Open Xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740989ED-457B-4B88-99DB-5FB8FD332AFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0D117-07CF-454C-B9CE-51120A4FD2BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="PCAN Read-Write Raw CAN Frame" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="InstrumentIdentifier">Instruments!$A$2:$A$22</definedName>
+    <definedName name="InstrumentIdentifier">Instruments!$A$2:$A$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -131,7 +131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -446,10 +446,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
@@ -485,7 +485,7 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
@@ -534,7 +534,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
@@ -597,7 +597,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -653,7 +653,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
added get ranges from sheet functionality
</commit_message>
<xml_diff>
--- a/Test Open Xml/test.xlsx
+++ b/Test Open Xml/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Open-Xml-LabVIEW\Test Open Xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0D117-07CF-454C-B9CE-51120A4FD2BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C0A95F-0F20-4D03-8088-BB541C244776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
   </bookViews>
@@ -20,7 +20,11 @@
     <sheet name="PCAN Read-Write Raw CAN Frame" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="InstrumentIdentifier">Instruments!$A$2:$A$6</definedName>
+    <definedName name="InstrumentClass" localSheetId="1">'CAN1'!$B$2</definedName>
+    <definedName name="InstrumentClass" localSheetId="2">'PCAN_USBBUS1  0x51'!$B$3</definedName>
+    <definedName name="InstrumentIdentifier" localSheetId="1">'CAN1'!$A$2</definedName>
+    <definedName name="InstrumentIdentifier" localSheetId="2">'PCAN_USBBUS1  0x51'!$A$3</definedName>
+    <definedName name="Instruments" localSheetId="0">Instruments!$A$2:$A$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,7 +95,7 @@
     <t>D:\git\HAL\HAL-Devices\Tests\resources\Triple-Sensor-NEO480.dbc</t>
   </si>
   <si>
-    <t>InstrumentIdentifier</t>
+    <t>Study Instruments</t>
   </si>
 </sst>
 </file>
@@ -446,7 +450,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +486,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change get named ranges of sheet to variant
</commit_message>
<xml_diff>
--- a/Test Open Xml/test.xlsx
+++ b/Test Open Xml/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Open-Xml-LabVIEW\Test Open Xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C0A95F-0F20-4D03-8088-BB541C244776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68656DF5-9249-4F4C-870E-39CD5E257A8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>InstrumentIdenfifier</t>
   </si>
@@ -47,9 +47,6 @@
     <t>ConfigureClass</t>
   </si>
   <si>
-    <t>gRPC XNET Read Raw CAN Frame</t>
-  </si>
-  <si>
     <t>CAN1</t>
   </si>
   <si>
@@ -96,6 +93,12 @@
   </si>
   <si>
     <t>Study Instruments</t>
+  </si>
+  <si>
+    <t>Attributes.ReadRate</t>
+  </si>
+  <si>
+    <t>Attributes.Baudrate</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -151,7 +154,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -449,11 +452,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D01127-9042-43DB-88ED-2CED71DAE784}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
@@ -463,17 +466,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -483,21 +486,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328F58-C35F-4796-8D47-99EF4FF1A847}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
     <col min="3" max="3" width="52.42578125" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,21 +512,27 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
+      <c r="D2">
+        <v>500000</v>
+      </c>
+      <c r="E2">
+        <v>10.5</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +548,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
@@ -557,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,21 +581,21 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -601,7 +611,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -612,19 +622,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -635,13 +645,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -657,17 +667,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,7 +688,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
polished boolean and tests
</commit_message>
<xml_diff>
--- a/Test Open Xml/test.xlsx
+++ b/Test Open Xml/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Open-Xml-LabVIEW\Test Open Xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68656DF5-9249-4F4C-870E-39CD5E257A8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A019A867-ADA6-4EC9-B8F0-C64944820F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>InstrumentIdenfifier</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Attributes.Baudrate</t>
+  </si>
+  <si>
+    <t>Attributes.Boolean</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328F58-C35F-4796-8D47-99EF4FF1A847}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,9 +502,10 @@
     <col min="3" max="3" width="52.42578125" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,8 +521,11 @@
       <c r="E1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -533,6 +540,9 @@
       </c>
       <c r="E2">
         <v>10.5</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get named ranges of sheet return cluster of 2d arrays instead of 3d array. corrected test herefore
</commit_message>
<xml_diff>
--- a/Test Open Xml/test.xlsx
+++ b/Test Open Xml/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Open-Xml-LabVIEW\Test Open Xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A019A867-ADA6-4EC9-B8F0-C64944820F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC69F3ED-6DCA-45BD-9BFC-9B03CF2D993B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>InstrumentIdenfifier</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Attributes.Boolean</t>
+  </si>
+  <si>
+    <t>#CAN1</t>
+  </si>
+  <si>
+    <t>#PCAN_USBBUS1  0x51</t>
   </si>
 </sst>
 </file>
@@ -455,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D01127-9042-43DB-88ED-2CED71DAE784}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,12 +480,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -491,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328F58-C35F-4796-8D47-99EF4FF1A847}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added test for get named range (var)
</commit_message>
<xml_diff>
--- a/Test Open Xml/test.xlsx
+++ b/Test Open Xml/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Open-Xml-LabVIEW\Test Open Xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC69F3ED-6DCA-45BD-9BFC-9B03CF2D993B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615CDF6E-06CB-4387-B416-A7192613CD75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{14239EE9-6B9F-42E8-A82B-812BD1501FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="PCAN Read-Write Raw CAN Frame" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="Attributes.Enabled">'CAN1'!$F$2</definedName>
+    <definedName name="Attributes.ReadRate">'CAN1'!$E$2</definedName>
     <definedName name="InstrumentClass" localSheetId="1">'CAN1'!$B$2</definedName>
     <definedName name="InstrumentClass" localSheetId="2">'PCAN_USBBUS1  0x51'!$B$3</definedName>
     <definedName name="InstrumentIdentifier" localSheetId="1">'CAN1'!$A$2</definedName>
@@ -101,13 +103,13 @@
     <t>Attributes.Baudrate</t>
   </si>
   <si>
-    <t>Attributes.Boolean</t>
-  </si>
-  <si>
     <t>#CAN1</t>
   </si>
   <si>
     <t>#PCAN_USBBUS1  0x51</t>
+  </si>
+  <si>
+    <t>Attributes.Enabled</t>
   </si>
 </sst>
 </file>
@@ -461,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D01127-9042-43DB-88ED-2CED71DAE784}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -480,12 +482,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -497,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7328F58-C35F-4796-8D47-99EF4FF1A847}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +530,7 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>